<commit_message>
Actualizacion de documentos y actualizacion del software
actualizado el area de gestion de proyectos, gestion de requisitoos, y creacion de la carpeta modelamiento de bases de datos
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/diseño y gestion de requisitos/Requerimientos funcionales y no funcionales.xlsx
+++ b/Fase 2/Evidencias Proyecto/diseño y gestion de requisitos/Requerimientos funcionales y no funcionales.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="191">
   <si>
     <t>categoria del requerimiento</t>
   </si>
@@ -216,9 +216,6 @@
     <t>manager-3.pdf</t>
   </si>
   <si>
-    <t>El manager 3 no se donde aplicarlo, Raúl</t>
-  </si>
-  <si>
     <t>MANAGER-4</t>
   </si>
   <si>
@@ -312,6 +309,9 @@
     <t>un usuario profesor podra crear una clase sincronica para que los alumnos inscritos asistan a la clase</t>
   </si>
   <si>
+    <t>usaremos el administrador de Django por ahora</t>
+  </si>
+  <si>
     <t>CLASS-2</t>
   </si>
   <si>
@@ -390,6 +390,9 @@
     <t>el sistema bloqueara el uso del modulo de clases a todos aquellos usuarios que no sean Usuarios alumnos mediante una membresia premium, el usuario puede preferir pagar directamente o usar la membresia premium por 3 meses de prueba de forma gratuita</t>
   </si>
   <si>
+    <t>Membresia-1.jpeg</t>
+  </si>
+  <si>
     <t>MEMBER-2</t>
   </si>
   <si>
@@ -397,6 +400,9 @@
   </si>
   <si>
     <t>el sistema desplegara informacion sobre los beneficios de la membresia premium frente a la licencia gratuita</t>
+  </si>
+  <si>
+    <t>membresia 3.jpeg</t>
   </si>
   <si>
     <t>MEMBER-3</t>
@@ -488,12 +494,111 @@
   <si>
     <t>tiene mockup?</t>
   </si>
+  <si>
+    <t>SYSTEM-001</t>
+  </si>
+  <si>
+    <t>Tiempo de carga</t>
+  </si>
+  <si>
+    <t>La duración que tendrá el sistema para cargar de pestaña a pestaña dentro del mismo</t>
+  </si>
+  <si>
+    <t>SYSTEM-002</t>
+  </si>
+  <si>
+    <t>Escalabilidad</t>
+  </si>
+  <si>
+    <t>El sistema mejora la calidad del trabajo distribuyendo de mejor manera la carga del trabajo.</t>
+  </si>
+  <si>
+    <t>SYSTEM-003</t>
+  </si>
+  <si>
+    <t>Autenticación y autorización</t>
+  </si>
+  <si>
+    <t>La funcionalidad del sistema tiene para reconocer usuarios y sus contraseñas de manera automática.</t>
+  </si>
+  <si>
+    <t>SYSTEM-004</t>
+  </si>
+  <si>
+    <t>Protección de datos sensibles</t>
+  </si>
+  <si>
+    <t>El sistema cuenta con la seguridad automática de poder proteger la información personal de todos los usuarios registrados en la página.</t>
+  </si>
+  <si>
+    <t>SYSTEM-005</t>
+  </si>
+  <si>
+    <t>Diseño intuitivo</t>
+  </si>
+  <si>
+    <t>Diseño simple y fácil de entender para cualquiera que entre a la página.</t>
+  </si>
+  <si>
+    <t>SYSTEM-006</t>
+  </si>
+  <si>
+    <t>Accesibilidad</t>
+  </si>
+  <si>
+    <t>El sistema es bastante facil de usar y es completamente libre de utilizar por el usuario.</t>
+  </si>
+  <si>
+    <t>SYSTEM-007</t>
+  </si>
+  <si>
+    <t>Soporte en vivo</t>
+  </si>
+  <si>
+    <t>El Sistema cuenta con un soporte online para evitar la caída del mismo.</t>
+  </si>
+  <si>
+    <t>SYSTEM-008</t>
+  </si>
+  <si>
+    <t>Transmisión de video en vivo</t>
+  </si>
+  <si>
+    <t>Utiliza funciones de soporte durante las transmisiones en vivo para impedir que estas se caigan durante las clases</t>
+  </si>
+  <si>
+    <t>SYSTEM-009</t>
+  </si>
+  <si>
+    <t>Soporte de audio y video</t>
+  </si>
+  <si>
+    <t>El sistema cuenta con un soporte online para evitar la caída del audio y el video de los archivos multimedi que lo tengan</t>
+  </si>
+  <si>
+    <t>SYSTEM-010</t>
+  </si>
+  <si>
+    <t>Mantenimiento continuo</t>
+  </si>
+  <si>
+    <t>Mantenimiento constante a la página para mantener su operación constantemente operativo.</t>
+  </si>
+  <si>
+    <t>SYSTEM-011</t>
+  </si>
+  <si>
+    <t>Compatibilidad entre navegadores</t>
+  </si>
+  <si>
+    <t>El sistema cuenta con una compatibilidad completa para operar en los navegadores de internet como Google Chrome o Microsoft Edge</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -540,6 +645,16 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -555,7 +670,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
     <border>
       <left style="thin">
@@ -571,11 +686,16 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -607,7 +727,31 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1442,7 +1586,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>16</v>
@@ -1456,9 +1600,7 @@
       <c r="K13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="L13" s="3"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1481,13 +1623,13 @@
         <v>54</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>14</v>
@@ -1526,16 +1668,16 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>14</v>
@@ -1550,7 +1692,7 @@
         <v>16</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -1574,16 +1716,16 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>14</v>
@@ -1598,7 +1740,7 @@
         <v>16</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -1622,16 +1764,16 @@
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>14</v>
@@ -1646,7 +1788,7 @@
         <v>16</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -1670,16 +1812,16 @@
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>14</v>
@@ -1694,7 +1836,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1718,16 +1860,16 @@
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>14</v>
@@ -1766,16 +1908,16 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>14</v>
@@ -1790,7 +1932,7 @@
         <v>16</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1814,16 +1956,16 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>15</v>
@@ -1837,10 +1979,13 @@
       <c r="H21" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I21" s="10" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>97</v>
@@ -1866,7 +2011,7 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>100</v>
@@ -1892,7 +2037,7 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>103</v>
@@ -1941,6 +2086,9 @@
       <c r="H25" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I25" s="10" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
@@ -1967,6 +2115,9 @@
       <c r="H26" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I26" s="10" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
@@ -2019,6 +2170,9 @@
       <c r="H28" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I28" s="11" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
@@ -2034,18 +2188,20 @@
         <v>122</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="4"/>
+      <c r="I29" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -2071,27 +2227,29 @@
         <v>119</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="4"/>
+      <c r="I30" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -2117,13 +2275,13 @@
         <v>119</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>15</v>
@@ -2163,13 +2321,13 @@
         <v>119</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>15</v>
@@ -2206,14 +2364,14 @@
     </row>
     <row r="33" ht="15.75" hidden="1" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>15</v>
@@ -2247,14 +2405,14 @@
     </row>
     <row r="34" ht="15.75" hidden="1" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>15</v>
@@ -2288,14 +2446,14 @@
     </row>
     <row r="35" ht="15.75" hidden="1" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>15</v>
@@ -2330,14 +2488,14 @@
     </row>
     <row r="36" ht="15.75" hidden="1" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>15</v>
@@ -2372,14 +2530,14 @@
     </row>
     <row r="37" ht="15.75" hidden="1" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>15</v>
@@ -2414,11 +2572,11 @@
     </row>
     <row r="38" ht="15.75" hidden="1" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
@@ -2454,11 +2612,11 @@
     </row>
     <row r="39" ht="15.75" hidden="1" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
@@ -2494,11 +2652,11 @@
     </row>
     <row r="40" ht="15.75" hidden="1" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
@@ -2534,11 +2692,11 @@
     </row>
     <row r="41" ht="15.75" hidden="1" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
@@ -2573,9 +2731,9 @@
       <c r="AB41" s="4"/>
     </row>
     <row r="42">
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -2599,9 +2757,9 @@
       <c r="AB42" s="4"/>
     </row>
     <row r="43">
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
@@ -2625,9 +2783,9 @@
       <c r="AB43" s="4"/>
     </row>
     <row r="44">
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -2651,9 +2809,9 @@
       <c r="AB44" s="4"/>
     </row>
     <row r="45">
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -2677,9 +2835,9 @@
       <c r="AB45" s="4"/>
     </row>
     <row r="46">
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
@@ -2703,9 +2861,9 @@
       <c r="AB46" s="4"/>
     </row>
     <row r="47">
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -2729,9 +2887,9 @@
       <c r="AB47" s="4"/>
     </row>
     <row r="48">
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
@@ -2755,9 +2913,9 @@
       <c r="AB48" s="4"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -2781,9 +2939,9 @@
       <c r="AB49" s="4"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
@@ -31548,11 +31706,13 @@
     <hyperlink r:id="rId16" ref="I18"/>
     <hyperlink r:id="rId17" ref="I19"/>
     <hyperlink r:id="rId18" ref="I20"/>
+    <hyperlink r:id="rId19" ref="I29"/>
+    <hyperlink r:id="rId20" ref="I30"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -31566,6 +31726,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="37.0"/>
+    <col customWidth="1" min="4" max="4" width="70.57"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -31581,11 +31745,177 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="2">
+      <c r="B2" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14">
+      <c r="D14" s="17"/>
+    </row>
+    <row r="20">
+      <c r="C20" s="18"/>
+    </row>
+    <row r="23">
+      <c r="C23" s="18"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>